<commit_message>
Added new actions and results
Matrix fixed 1\5
</commit_message>
<xml_diff>
--- a/Plan_Deystviy (1).xlsx
+++ b/Plan_Deystviy (1).xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>№#</t>
   </si>
@@ -57,28 +57,7 @@
     <t>A2.3</t>
   </si>
   <si>
-    <t>A2.13</t>
-  </si>
-  <si>
-    <t>A2.17</t>
-  </si>
-  <si>
     <t>A1.6</t>
-  </si>
-  <si>
-    <t>A1.7</t>
-  </si>
-  <si>
-    <t>A1.8</t>
-  </si>
-  <si>
-    <t>A1.9</t>
-  </si>
-  <si>
-    <t>A1.10</t>
-  </si>
-  <si>
-    <t>A1.11</t>
   </si>
   <si>
     <r>
@@ -243,12 +222,48 @@
   <si>
     <t>Разработке программного продукта IT Платформы группой программистов</t>
   </si>
+  <si>
+    <t>A2.4</t>
+  </si>
+  <si>
+    <t>A2.5</t>
+  </si>
+  <si>
+    <t>A3.1</t>
+  </si>
+  <si>
+    <t>A3.2</t>
+  </si>
+  <si>
+    <t>A3.3</t>
+  </si>
+  <si>
+    <t>A3.4</t>
+  </si>
+  <si>
+    <t>A3.5</t>
+  </si>
+  <si>
+    <t>A4.1</t>
+  </si>
+  <si>
+    <t>A4.2</t>
+  </si>
+  <si>
+    <t>A4.3</t>
+  </si>
+  <si>
+    <t>A4.4</t>
+  </si>
+  <si>
+    <t>A4.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,28 +711,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="49.90625" customWidth="1"/>
-    <col min="5" max="5" width="91.6328125" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" customWidth="1"/>
+    <col min="5" max="5" width="91.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="18">
+    <row r="2" spans="2:5" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -725,222 +741,232 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="35.5">
+    <row r="4" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="54">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="54" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="72">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="72" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="79.5" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:5" ht="54">
+    <row r="10" spans="2:5" ht="54" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:5" ht="53">
+    <row r="11" spans="2:5" ht="52.8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:5" s="16" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:5" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="2:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:5" ht="69.599999999999994" x14ac:dyDescent="0.35">
+      <c r="B17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" s="13" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="2:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="B19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="72">
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:5" s="16" customFormat="1" ht="54">
-      <c r="B13" s="5"/>
-      <c r="C13" s="11" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="2:5" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="2:5" ht="90" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="2:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="2:5" s="16" customFormat="1" ht="36">
-      <c r="B14" s="5"/>
-      <c r="C14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="2:5" ht="36">
-      <c r="B15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" ht="72">
-      <c r="B16" s="5"/>
-      <c r="C16" s="11" t="s">
+    </row>
+    <row r="24" spans="2:5" ht="90" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="B25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" ht="70">
-      <c r="B17" s="17" t="s">
+    </row>
+    <row r="26" spans="2:5" ht="90" x14ac:dyDescent="0.35">
+      <c r="B26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="20" t="s">
+    </row>
+    <row r="27" spans="2:5" ht="52.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" s="13" customFormat="1" ht="54">
-      <c r="B18" s="10"/>
-      <c r="C18" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="2:5" ht="54">
-      <c r="B19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="2:5" ht="37" customHeight="1">
-      <c r="B20" s="5"/>
-      <c r="C20" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" ht="90">
-      <c r="B21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" ht="51" customHeight="1">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="58.5" customHeight="1">
-      <c r="B23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="90">
-      <c r="B24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="54">
-      <c r="B25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="90">
-      <c r="B26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="53" customHeight="1">
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="90" customHeight="1">
-      <c r="B28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="18">
+    </row>
+    <row r="29" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="2:5" ht="18">
+    <row r="30" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:5" ht="18">
+    <row r="31" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="2:5" ht="18">
+    <row r="32" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
     </row>

</xml_diff>

<commit_message>
LOGIC TABLE IS DONE
</commit_message>
<xml_diff>
--- a/Plan_Deystviy (1).xlsx
+++ b/Plan_Deystviy (1).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>№#</t>
   </si>
@@ -125,9 +125,6 @@
     <t>R3</t>
   </si>
   <si>
-    <t>IT Платформы для достижения Целей и Обьективов Проекта  совместно с Партнерами создана, принята к эсплуатации и сопровождению</t>
-  </si>
-  <si>
     <t>Совместно с пратнерами, создание   согласованного  функционала будущей IT Платформы</t>
   </si>
   <si>
@@ -258,12 +255,39 @@
   <si>
     <t>A4.5</t>
   </si>
+  <si>
+    <t>Обеспечение комфорта партнёров (вода,  еда, кофе)</t>
+  </si>
+  <si>
+    <t>Затраты на концелярию</t>
+  </si>
+  <si>
+    <t>1500*мес</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 специалиста с зп по 500 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 аренда офиса, </t>
+  </si>
+  <si>
+    <t>Создание IT Платформы для достижения Целей и Обьективов Проекта  совместно с Партнерами создана, принята к эсплуатации и сопровождению</t>
+  </si>
+  <si>
+    <t>Наем спец. по аналитике и анализу данных</t>
+  </si>
+  <si>
+    <t>550*3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Затраты на канцелярию </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +362,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +401,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -417,9 +487,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -438,6 +505,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,238 +801,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E32"/>
+  <dimension ref="B2:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="49.88671875" customWidth="1"/>
-    <col min="5" max="5" width="91.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24">
+        <v>30</v>
+      </c>
+      <c r="H6" s="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="36" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="72" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="211.2" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="2:5" ht="52.8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="52.8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:5" s="16" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" s="15" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="2:5" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="2:12" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="2:5" ht="36" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="2:12" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="142.80000000000001" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" ht="72" x14ac:dyDescent="0.35">
-      <c r="B16" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" ht="69.599999999999994" x14ac:dyDescent="0.35">
-      <c r="B17" s="17" t="s">
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" s="13" customFormat="1" ht="211.2" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" s="13" customFormat="1" ht="54" x14ac:dyDescent="0.35">
-      <c r="B18" s="10" t="s">
+      <c r="D18" s="13">
+        <v>100</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="71.400000000000006" x14ac:dyDescent="0.35">
+      <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="2:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="B19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="4"/>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="2:5" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>2020</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="2:5" ht="90" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="2:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="90" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>29</v>
+        <v>46</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="54" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="90" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>27</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="52.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="18" x14ac:dyDescent="0.35">

</xml_diff>